<commit_message>
fixed bugs, new disparity formula
</commit_message>
<xml_diff>
--- a/Calibration/data4_plot.xlsx
+++ b/Calibration/data4_plot.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPadP50\Documents\ObjDetection\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AD496A6-59C3-425B-AB43-098D9A3933E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D357BDFF-073F-4CF5-8DAF-83519BE0C8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet!$A$1:$A$35</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet!$B$1:$B$35</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,6 +30,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+  <si>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>Cone 2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,6 +451,552 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0384-45E3-9B5B-237ADD56140B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1007521840"/>
+        <c:axId val="1007509360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1007521840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1007509360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1007509360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1007521840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.9167465617839264E-2"/>
+          <c:y val="9.6052539817382265E-2"/>
+          <c:w val="0.93565677819420079"/>
+          <c:h val="0.84387055175617365"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8968262948330357E-2"/>
+                  <c:y val="-0.68814628180098991"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet (2)'!$A$2:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>0.68807799999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67742000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64877499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63990100000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63671800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62008099999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61188200000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60619199999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59292999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58531</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57691899999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57257899999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.56182399999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.55594100000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54885200000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.51215200000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.49310300000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.51331000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5027488</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.49657600000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.48712299999999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.48668899999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47911799999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.47762300000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.46373399999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.45900800000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.45394400000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.44362400000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.44232199999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.43610100000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.43856000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.426311</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.42211599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet (2)'!$B$2:$B$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>163.19499999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>177.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.42000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>193.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>208.28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>215.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>223.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>231.14000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>238.76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>246.38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>266.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>279.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>287.02</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>304.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>317.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>342.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>355.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>368.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>393.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>406.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>431.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>457.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>482.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>533.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>558.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>584.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>609.6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D85B-4BC7-B3B1-5047F65AE589}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -673,7 +1227,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1214,6 +2324,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D3ADD4-B669-45BF-AABA-3B799B634873}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1517,7 +2670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -2101,4 +3254,727 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D5BA9A-F327-4BA6-9289-303E7A3FC05A}">
+  <dimension ref="A1:O77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="9.3046875" customWidth="1"/>
+    <col min="15" max="15" width="12.4609375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>0.68807799999999997</v>
+      </c>
+      <c r="B2">
+        <f>C2*2.54</f>
+        <v>163.19499999999999</v>
+      </c>
+      <c r="C2">
+        <v>64.25</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.229383680555556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>0.67742000000000002</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B16" si="0">C3*2.54</f>
+        <v>170.18</v>
+      </c>
+      <c r="C3">
+        <v>67</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>0.64877499999999999</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>177.8</v>
+      </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>0.63990100000000005</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>185.42000000000002</v>
+      </c>
+      <c r="C5">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>0.63671800000000001</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>193.04</v>
+      </c>
+      <c r="C6">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>0.62008099999999999</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>200.66</v>
+      </c>
+      <c r="C7">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>0.61188200000000004</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>208.28</v>
+      </c>
+      <c r="C8">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>0.60619199999999995</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>215.9</v>
+      </c>
+      <c r="C9">
+        <v>85</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>0.59292999999999996</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>223.52</v>
+      </c>
+      <c r="C10">
+        <v>88</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>0.58531</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>231.14000000000001</v>
+      </c>
+      <c r="C11">
+        <v>91</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>0.57691899999999996</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>238.76</v>
+      </c>
+      <c r="C12">
+        <v>94</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>0.57257899999999995</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>246.38</v>
+      </c>
+      <c r="C13">
+        <v>97</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>0.56182399999999999</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>0.55594100000000002</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>266.7</v>
+      </c>
+      <c r="C15">
+        <v>105</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>0.54885200000000001</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>279.39999999999998</v>
+      </c>
+      <c r="C16">
+        <v>110</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>0.51215200000000005</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:B23" si="1">C17*2.54</f>
+        <v>287.02</v>
+      </c>
+      <c r="C17">
+        <v>113</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>0.49310300000000001</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>304.8</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>0.51331000000000004</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>317.5</v>
+      </c>
+      <c r="C19">
+        <v>125</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>0.5027488</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>342.9</v>
+      </c>
+      <c r="C20">
+        <v>135</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>0.49657600000000002</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>355.6</v>
+      </c>
+      <c r="C21">
+        <v>140</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>0.48712299999999997</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>368.3</v>
+      </c>
+      <c r="C22">
+        <v>145</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>0.48668899999999998</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>381</v>
+      </c>
+      <c r="C23">
+        <v>150</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>0.47911799999999999</v>
+      </c>
+      <c r="B24">
+        <f>C24*2.54</f>
+        <v>393.7</v>
+      </c>
+      <c r="C24">
+        <v>155</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>0.47762300000000002</v>
+      </c>
+      <c r="B25">
+        <f>C25*2.54</f>
+        <v>406.4</v>
+      </c>
+      <c r="C25">
+        <v>160</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>0.46373399999999998</v>
+      </c>
+      <c r="B26">
+        <f>C26*2.54</f>
+        <v>431.8</v>
+      </c>
+      <c r="C26">
+        <v>170</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>0.45900800000000003</v>
+      </c>
+      <c r="B27">
+        <f>C27*2.54</f>
+        <v>457.2</v>
+      </c>
+      <c r="C27">
+        <v>180</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>0.45394400000000001</v>
+      </c>
+      <c r="B28">
+        <f>C28*2.54</f>
+        <v>482.6</v>
+      </c>
+      <c r="C28">
+        <v>190</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>0.44362400000000002</v>
+      </c>
+      <c r="B29">
+        <f>C29*2.54</f>
+        <v>508</v>
+      </c>
+      <c r="C29">
+        <v>200</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>0.44232199999999999</v>
+      </c>
+      <c r="B30">
+        <f>C30*2.54</f>
+        <v>533.4</v>
+      </c>
+      <c r="C30">
+        <v>210</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>0.43610100000000002</v>
+      </c>
+      <c r="B31">
+        <f>C31*2.54</f>
+        <v>558.79999999999995</v>
+      </c>
+      <c r="C31">
+        <v>220</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>0.43856000000000001</v>
+      </c>
+      <c r="B32">
+        <f>C32*2.54</f>
+        <v>584.20000000000005</v>
+      </c>
+      <c r="C32">
+        <v>230</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>0.426311</v>
+      </c>
+      <c r="B33">
+        <f>C33*2.54</f>
+        <v>609.6</v>
+      </c>
+      <c r="C33">
+        <v>240</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>0.42211599999999999</v>
+      </c>
+      <c r="B34">
+        <f>C34*2.54</f>
+        <v>635</v>
+      </c>
+      <c r="C34">
+        <v>250</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="D35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="D36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="O37">
+        <f>(-2480*F2^3)+(3903.8*F2^2)-(2030.7*F2)+432.33</f>
+        <v>141.99406746672639</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G43">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G44">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G46">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G47">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="G48">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G49">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G50">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G51">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G52">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G53">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G54">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G55">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G56">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G57">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G58">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G59">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G60">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G61">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G62">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G63">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G64">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G65">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G66">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G67">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G68">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G69">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G70">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G71">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G72">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G73">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G74">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G75">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G76">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G77">
+        <v>377</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>